<commit_message>
AddFodstuff comp  is inserting new foodstuff into foodstuffs alphabetically in handleSubmit
</commit_message>
<xml_diff>
--- a/lib/ingredients.xlsx
+++ b/lib/ingredients.xlsx
@@ -3394,7 +3394,7 @@
     <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>697</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="683" customHeight="1" ht="17.25">

</xml_diff>